<commit_message>
Pro monoos form Morris 2011 broken
</commit_message>
<xml_diff>
--- a/data/fig1&3_morris_2011.xlsx
+++ b/data/fig1&3_morris_2011.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkm/Documents/Talmy_research/Zinser_lab/Projects/ROS_focused/Project_3_Morris_2011_ROS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFCF0B1-58B4-344B-B099-048CD11FFB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD05FE2B-BDD7-6D4D-9103-725332D49250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="500" windowWidth="27120" windowHeight="16120" activeTab="2" xr2:uid="{04719FF1-348F-6349-832C-C1D7FD25A56E}"/>
+    <workbookView xWindow="3780" yWindow="1000" windowWidth="27120" windowHeight="16120" activeTab="1" xr2:uid="{04719FF1-348F-6349-832C-C1D7FD25A56E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="32">
   <si>
     <t>Strain</t>
   </si>
@@ -96,10 +96,7 @@
     <t>If you really need those data I can try harder to fish them out.</t>
   </si>
   <si>
-    <t>Tims (days)</t>
-  </si>
-  <si>
-    <t>Organism</t>
+    <t>H</t>
   </si>
   <si>
     <t>P</t>
@@ -109,6 +106,33 @@
   </si>
   <si>
     <t>Morris_2011_fig3</t>
+  </si>
+  <si>
+    <t>organism</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>0rganism</t>
+  </si>
+  <si>
+    <t>Treatment(HOOH (uM))</t>
+  </si>
+  <si>
+    <t>Morris_2011_fig1</t>
+  </si>
+  <si>
+    <t>rep1</t>
+  </si>
+  <si>
+    <t>rep2</t>
+  </si>
+  <si>
+    <t>rep3</t>
   </si>
 </sst>
 </file>
@@ -2605,935 +2629,1536 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CEA5292-E783-2C45-9D37-CBAA1C3A7F23}">
-  <dimension ref="A3:K32"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>106351</v>
+      </c>
+      <c r="F2" s="2">
+        <v>117613</v>
+      </c>
+      <c r="G2" s="2">
+        <v>120264.2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.22013888888614019</v>
+      </c>
+      <c r="E3" s="2">
+        <v>87181.4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>95532.2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>95322.6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.22013888888614019</v>
-      </c>
-      <c r="G4" s="1">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
         <v>0.49583333333430302</v>
       </c>
-      <c r="H4" s="1">
-        <v>0.9881944444423425</v>
-      </c>
-      <c r="I4" s="1">
-        <v>2.1263888888861402</v>
-      </c>
-      <c r="J4" s="1">
-        <v>4.0749999999970896</v>
-      </c>
-      <c r="K4">
-        <v>7.0999999999985448</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E4" s="2">
+        <v>124319.4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>138061.6</v>
+      </c>
+      <c r="G4" s="2">
+        <v>130595.6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" s="1">
+        <v>0.9881944444423425</v>
       </c>
       <c r="E5" s="2">
-        <v>106351</v>
+        <v>156087</v>
       </c>
       <c r="F5" s="2">
-        <v>87181.4</v>
+        <v>158292.20000000001</v>
       </c>
       <c r="G5" s="2">
-        <v>124319.4</v>
-      </c>
-      <c r="H5" s="2">
-        <v>156087</v>
-      </c>
-      <c r="I5" s="2">
-        <v>24438.6</v>
-      </c>
-      <c r="J5" s="2">
-        <v>678.8</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1696.1079999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>164541.6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6">
-        <v>2</v>
+      <c r="D6" s="1">
+        <v>2.1263888888861402</v>
       </c>
       <c r="E6" s="2">
-        <v>117613</v>
+        <v>24438.6</v>
       </c>
       <c r="F6" s="2">
-        <v>95532.2</v>
+        <v>34281.199999999997</v>
       </c>
       <c r="G6" s="2">
-        <v>138061.6</v>
-      </c>
-      <c r="H6" s="2">
-        <v>158292.20000000001</v>
-      </c>
-      <c r="I6" s="2">
-        <v>34281.199999999997</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1018.22</v>
-      </c>
-      <c r="K6" s="2">
-        <v>339.22039999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>43956</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
-        <v>3</v>
+      <c r="D7" s="1">
+        <v>4.0749999999970896</v>
       </c>
       <c r="E7" s="2">
-        <v>120264.2</v>
+        <v>678.8</v>
       </c>
       <c r="F7" s="2">
-        <v>95322.6</v>
+        <v>1018.22</v>
       </c>
       <c r="G7" s="2">
-        <v>130595.6</v>
-      </c>
-      <c r="H7" s="2">
-        <v>164541.6</v>
-      </c>
-      <c r="I7" s="2">
-        <v>43956</v>
-      </c>
-      <c r="J7" s="2">
         <v>678.45600000000002</v>
       </c>
-      <c r="K7" s="2">
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>7.0999999999985448</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1696.1079999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>339.22039999999998</v>
+      </c>
+      <c r="G8" s="2">
         <v>1356.8520000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>97701.2</v>
-      </c>
-      <c r="F8" s="2">
-        <v>95655.2</v>
-      </c>
-      <c r="G8" s="2">
-        <v>139759.4</v>
-      </c>
-      <c r="H8" s="2">
-        <v>159381</v>
-      </c>
-      <c r="I8" s="2">
-        <v>201290</v>
-      </c>
-      <c r="J8" s="2">
-        <v>228682.8</v>
-      </c>
-      <c r="K8" s="2">
-        <v>193368.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9">
-        <v>2</v>
+      <c r="D9" s="1">
+        <v>0</v>
       </c>
       <c r="E9" s="2">
+        <v>97701.2</v>
+      </c>
+      <c r="F9" s="2">
         <v>106015.2</v>
       </c>
-      <c r="F9" s="2">
-        <v>91584.8</v>
-      </c>
       <c r="G9" s="2">
-        <v>128974.6</v>
-      </c>
-      <c r="H9" s="2">
-        <v>161843.20000000001</v>
-      </c>
-      <c r="I9" s="2">
-        <v>190601.8</v>
-      </c>
-      <c r="J9" s="2">
-        <v>186596</v>
-      </c>
-      <c r="K9" s="2">
-        <v>128586.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>112463.4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D10">
-        <v>3</v>
+      <c r="D10" s="1">
+        <v>0.22013888888614019</v>
       </c>
       <c r="E10" s="2">
-        <v>112463.4</v>
+        <v>95655.2</v>
       </c>
       <c r="F10" s="2">
+        <v>91584.8</v>
+      </c>
+      <c r="G10" s="2">
         <v>90226.8</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.49583333333430302</v>
+      </c>
+      <c r="E11" s="2">
+        <v>139759.4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>128974.6</v>
+      </c>
+      <c r="G11" s="2">
         <v>133482.6</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.9881944444423425</v>
+      </c>
+      <c r="E12" s="2">
+        <v>159381</v>
+      </c>
+      <c r="F12" s="2">
+        <v>161843.20000000001</v>
+      </c>
+      <c r="G12" s="2">
         <v>165900.4</v>
       </c>
-      <c r="I10" s="2">
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2.1263888888861402</v>
+      </c>
+      <c r="E13" s="2">
+        <v>201290</v>
+      </c>
+      <c r="F13" s="2">
+        <v>190601.8</v>
+      </c>
+      <c r="G13" s="2">
         <v>195186.2</v>
       </c>
-      <c r="J10" s="2">
-        <v>231504</v>
-      </c>
-      <c r="K10" s="2">
-        <v>218485.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>97583</v>
-      </c>
-      <c r="F11" s="2">
-        <v>85137.2</v>
-      </c>
-      <c r="G11" s="2">
-        <v>128121.2</v>
-      </c>
-      <c r="H11" s="2">
-        <v>166423.6</v>
-      </c>
-      <c r="I11" s="2">
-        <v>216838</v>
-      </c>
-      <c r="J11" s="2">
-        <v>237471.6</v>
-      </c>
-      <c r="K11" s="2">
-        <v>264293.59999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2">
-        <v>99113.4</v>
-      </c>
-      <c r="F12" s="2">
-        <v>94980.6</v>
-      </c>
-      <c r="G12" s="2">
-        <v>133888.6</v>
-      </c>
-      <c r="H12" s="2">
-        <v>171932</v>
-      </c>
-      <c r="I12" s="2">
-        <v>198238.6</v>
-      </c>
-      <c r="J12" s="2">
-        <v>199825.2</v>
-      </c>
-      <c r="K12" s="2">
-        <v>187605.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13" s="2">
-        <v>99225.2</v>
-      </c>
-      <c r="F13" s="2">
-        <v>92721.4</v>
-      </c>
-      <c r="G13" s="2">
-        <v>128463.2</v>
-      </c>
-      <c r="H13" s="2">
-        <v>161749.20000000001</v>
-      </c>
-      <c r="I13" s="2">
-        <v>195867.6</v>
-      </c>
-      <c r="J13" s="2">
-        <v>184894.8</v>
-      </c>
-      <c r="K13" s="2">
-        <v>200257.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D14">
-        <v>1</v>
+      <c r="D14" s="1">
+        <v>4.0749999999970896</v>
       </c>
       <c r="E14" s="2">
-        <v>98719.6</v>
+        <v>228682.8</v>
       </c>
       <c r="F14" s="2">
-        <v>84123.4</v>
+        <v>186596</v>
       </c>
       <c r="G14" s="2">
-        <v>106857.60000000001</v>
-      </c>
-      <c r="H14" s="2">
-        <v>133345.60000000001</v>
-      </c>
-      <c r="I14" s="2">
-        <v>179050</v>
-      </c>
-      <c r="J14" s="2">
-        <v>211698.8</v>
-      </c>
-      <c r="K14" s="2">
-        <v>170996.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>231504</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>7.0999999999985448</v>
       </c>
       <c r="E15" s="2">
-        <v>95160.2</v>
+        <v>193368.8</v>
       </c>
       <c r="F15" s="2">
-        <v>75136.600000000006</v>
+        <v>128586.8</v>
       </c>
       <c r="G15" s="2">
-        <v>110985.4</v>
-      </c>
-      <c r="H15" s="2">
-        <v>137744</v>
-      </c>
-      <c r="I15" s="2">
-        <v>163774.6</v>
-      </c>
-      <c r="J15" s="2">
-        <v>190657.6</v>
-      </c>
-      <c r="K15" s="2">
-        <v>133321.20000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>218485.6</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16" s="2">
-        <v>104659</v>
-      </c>
-      <c r="F16" s="2">
-        <v>99223</v>
-      </c>
-      <c r="G16" s="2">
-        <v>132808.4</v>
-      </c>
-      <c r="H16" s="2">
-        <v>168970.4</v>
-      </c>
-      <c r="I16" s="2">
-        <v>205072</v>
-      </c>
-      <c r="J16" s="2">
-        <v>211138.4</v>
-      </c>
-      <c r="K16" s="2">
-        <v>146213.6</v>
+        <v>8</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>36.603252869686344</v>
+      </c>
+      <c r="F16" s="3">
+        <v>33.241843634639665</v>
+      </c>
+      <c r="G16" s="3">
+        <v>36.850566725415149</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.22013888888614019</v>
+      </c>
+      <c r="E17" s="3">
+        <v>269.77564385822836</v>
+      </c>
+      <c r="F17" s="3">
+        <v>254.49066199685433</v>
+      </c>
+      <c r="G17" s="3">
+        <v>253.68225480575279</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.49583333333430302</v>
+      </c>
+      <c r="E18" s="3">
+        <v>391.12965057082386</v>
+      </c>
+      <c r="F18" s="3">
+        <v>374.42355633580132</v>
+      </c>
+      <c r="G18" s="3">
+        <v>358.37990538827944</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.9881944444423425</v>
+      </c>
+      <c r="E19" s="3">
+        <v>398.20127586681849</v>
+      </c>
+      <c r="F19" s="3">
+        <v>370.02294231462724</v>
+      </c>
+      <c r="G19" s="3">
+        <v>369.73189585912348</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0.22013888888614019</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0.49583333333430346</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0.9881944444423425</v>
-      </c>
-      <c r="I20" s="1">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1">
         <v>2.1263888888861402</v>
       </c>
-      <c r="J20" s="1">
-        <v>4.0749999999970896</v>
-      </c>
-      <c r="K20" s="1">
-        <v>7.0999999999985448</v>
+      <c r="E20" s="3">
+        <v>860.7933817900323</v>
+      </c>
+      <c r="F20" s="3">
+        <v>634.02445362894582</v>
+      </c>
+      <c r="G20" s="3">
+        <v>792.85518614120065</v>
+      </c>
+      <c r="H20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D21">
-        <v>1</v>
+      <c r="D21" s="1">
+        <v>4.0749999999970896</v>
       </c>
       <c r="E21" s="3">
-        <v>36.603252869686344</v>
+        <v>2247.0488593365471</v>
       </c>
       <c r="F21" s="3">
-        <v>269.77564385822836</v>
+        <v>1987.7730846749801</v>
       </c>
       <c r="G21" s="3">
-        <v>391.12965057082386</v>
-      </c>
-      <c r="H21" s="3">
-        <v>398.20127586681849</v>
-      </c>
-      <c r="I21" s="3">
-        <v>860.7933817900323</v>
-      </c>
-      <c r="J21" s="3">
-        <v>2247.0488593365471</v>
-      </c>
-      <c r="K21" s="3">
-        <v>2963.909007386826</v>
-      </c>
+        <v>1838.0787497256465</v>
+      </c>
+      <c r="H21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>7.0999999999985448</v>
       </c>
       <c r="E22" s="3">
-        <v>33.241843634639665</v>
+        <v>2963.909007386826</v>
       </c>
       <c r="F22" s="3">
-        <v>254.49066199685433</v>
+        <v>2812.5436069437205</v>
       </c>
       <c r="G22" s="3">
-        <v>374.42355633580132</v>
-      </c>
-      <c r="H22" s="3">
-        <v>370.02294231462724</v>
-      </c>
-      <c r="I22" s="3">
-        <v>634.02445362894582</v>
-      </c>
-      <c r="J22" s="3">
-        <v>1987.7730846749801</v>
-      </c>
-      <c r="K22" s="3">
-        <v>2812.5436069437205</v>
-      </c>
+        <v>2749.476493825573</v>
+      </c>
+      <c r="H22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
       </c>
       <c r="E23" s="3">
-        <v>36.850566725415149</v>
+        <v>30.232384493930994</v>
       </c>
       <c r="F23" s="3">
-        <v>253.68225480575279</v>
+        <v>27.013772597100697</v>
       </c>
       <c r="G23" s="3">
-        <v>358.37990538827944</v>
-      </c>
-      <c r="H23" s="3">
-        <v>369.73189585912348</v>
-      </c>
-      <c r="I23" s="3">
-        <v>792.85518614120065</v>
-      </c>
-      <c r="J23" s="3">
-        <v>1838.0787497256465</v>
-      </c>
-      <c r="K23" s="3">
-        <v>2749.476493825573</v>
-      </c>
+        <v>28.296374637466982</v>
+      </c>
+      <c r="H23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
-      <c r="D24">
-        <v>1</v>
+      <c r="D24" s="1">
+        <v>0.22013888888614019</v>
       </c>
       <c r="E24" s="3">
-        <v>30.232384493930994</v>
+        <v>29.867512392315916</v>
       </c>
       <c r="F24" s="3">
-        <v>29.867512392315916</v>
+        <v>18.496396118129798</v>
       </c>
       <c r="G24" s="3">
-        <v>62.633194545330866</v>
-      </c>
-      <c r="H24" s="3">
-        <v>54.129026142708426</v>
-      </c>
-      <c r="I24" s="3">
-        <v>78.922325128002512</v>
-      </c>
-      <c r="J24" s="3">
-        <v>190.84165322753788</v>
-      </c>
-      <c r="K24" s="3">
-        <v>109.57430479599725</v>
-      </c>
+        <v>26.286456663309536</v>
+      </c>
+      <c r="H24" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
       </c>
-      <c r="D25">
-        <v>2</v>
+      <c r="D25" s="1">
+        <v>0.49583333333430302</v>
       </c>
       <c r="E25" s="3">
-        <v>27.013772597100697</v>
+        <v>62.633194545330866</v>
       </c>
       <c r="F25" s="3">
-        <v>18.496396118129837</v>
+        <v>53.623126510576526</v>
       </c>
       <c r="G25" s="3">
-        <v>53.623126510576526</v>
-      </c>
-      <c r="H25" s="3">
-        <v>49.160315437186512</v>
-      </c>
-      <c r="I25" s="3">
-        <v>75.891325552255012</v>
-      </c>
-      <c r="J25" s="3">
-        <v>150.79782500576502</v>
-      </c>
-      <c r="K25" s="3">
-        <v>115.95523278923417</v>
-      </c>
+        <v>49.870056828364966</v>
+      </c>
+      <c r="H25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
       </c>
-      <c r="D26">
-        <v>3</v>
+      <c r="D26" s="1">
+        <v>0.9881944444423425</v>
       </c>
       <c r="E26" s="3">
-        <v>28.296374637466982</v>
+        <v>54.129026142708426</v>
       </c>
       <c r="F26" s="3">
-        <v>26.286456663309536</v>
+        <v>49.160315437186512</v>
       </c>
       <c r="G26" s="3">
-        <v>49.870056828364966</v>
-      </c>
-      <c r="H26" s="3">
         <v>50.233926636119236</v>
       </c>
-      <c r="I26" s="3">
-        <v>69.814622187541204</v>
-      </c>
-      <c r="J26" s="3">
-        <v>134.15817699531411</v>
-      </c>
-      <c r="K26" s="3">
-        <v>89.767858018422487</v>
-      </c>
+      <c r="H26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2.1263888888861402</v>
       </c>
       <c r="E27" s="3">
-        <v>32.517560929232246</v>
+        <v>78.922325128002512</v>
       </c>
       <c r="F27" s="3">
-        <v>177.33507782715219</v>
+        <v>75.891325552255012</v>
       </c>
       <c r="G27" s="3">
-        <v>107.7330631891956</v>
-      </c>
-      <c r="H27" s="3">
-        <v>52.35138372647782</v>
-      </c>
-      <c r="I27" s="3">
-        <v>59.722880184432029</v>
-      </c>
-      <c r="J27" s="3">
-        <v>72.744060432708977</v>
-      </c>
-      <c r="K27" s="3">
-        <v>55.363535287553304</v>
-      </c>
+        <v>69.814622187541204</v>
+      </c>
+      <c r="H27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="D28" s="1">
+        <v>4.0749999999970896</v>
       </c>
       <c r="E28" s="3">
-        <v>31.569848726909015</v>
+        <v>190.84165322753788</v>
       </c>
       <c r="F28" s="3">
-        <v>178.98094596408873</v>
+        <v>150.79782500576502</v>
       </c>
       <c r="G28" s="3">
-        <v>103.17777356395095</v>
-      </c>
-      <c r="H28" s="3">
-        <v>51.228826711620684</v>
-      </c>
-      <c r="I28" s="3">
-        <v>60.79833766652871</v>
-      </c>
-      <c r="J28" s="3">
-        <v>68.866336044869058</v>
-      </c>
-      <c r="K28" s="3">
-        <v>47.838679734676361</v>
-      </c>
+        <v>134.15817699531411</v>
+      </c>
+      <c r="H28" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>7.0999999999985448</v>
       </c>
       <c r="E29" s="3">
-        <v>29.987914014251345</v>
+        <v>109.57430479599725</v>
       </c>
       <c r="F29" s="3">
-        <v>162.785507853838</v>
+        <v>115.95523278923417</v>
       </c>
       <c r="G29" s="3">
-        <v>108.10037164190248</v>
-      </c>
-      <c r="H29" s="3">
-        <v>55.731415543140315</v>
-      </c>
-      <c r="I29" s="3">
-        <v>59.160217355284772</v>
-      </c>
-      <c r="J29" s="3">
-        <v>69.17605375194168</v>
-      </c>
-      <c r="K29" s="3">
-        <v>49.598276915691713</v>
-      </c>
+        <v>89.767858018422487</v>
+      </c>
+      <c r="H29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3">
-        <v>19.644190831782375</v>
-      </c>
-      <c r="F30" s="3">
-        <v>-32.431813256435021</v>
-      </c>
-      <c r="G30" s="3">
-        <v>-32.235847570610247</v>
-      </c>
-      <c r="H30" s="3">
-        <v>-25.223472178409679</v>
-      </c>
-      <c r="I30" s="3">
-        <v>-35.296297536212876</v>
-      </c>
-      <c r="J30" s="3">
-        <v>33.955744488115272</v>
-      </c>
-      <c r="K30" s="3">
-        <v>-11.600473912886457</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>97583</v>
+      </c>
+      <c r="F30" s="2">
+        <v>99113.4</v>
+      </c>
+      <c r="G30" s="2">
+        <v>99225.2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-      <c r="E31" s="3">
-        <v>27.508879192945543</v>
-      </c>
-      <c r="F31" s="3">
-        <v>-7.8933458560227336</v>
-      </c>
-      <c r="G31" s="3">
-        <v>-27.371462065310538</v>
-      </c>
-      <c r="H31" s="3">
-        <v>-24.881561856139854</v>
-      </c>
-      <c r="I31" s="3">
-        <v>-33.85599422746742</v>
-      </c>
-      <c r="J31" s="3">
-        <v>22.526070565314484</v>
-      </c>
-      <c r="K31" s="3">
-        <v>-12.259599628150966</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.22013888888614019</v>
+      </c>
+      <c r="E31" s="2">
+        <v>85137.2</v>
+      </c>
+      <c r="F31" s="2">
+        <v>94980.6</v>
+      </c>
+      <c r="G31" s="2">
+        <v>92721.4</v>
+      </c>
+      <c r="H31" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.49583333333430302</v>
+      </c>
+      <c r="E32" s="2">
+        <v>128121.2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>133888.6</v>
+      </c>
+      <c r="G32" s="2">
+        <v>128463.2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>9</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.9881944444423425</v>
+      </c>
+      <c r="E33" s="2">
+        <v>166423.6</v>
+      </c>
+      <c r="F33" s="2">
+        <v>171932</v>
+      </c>
+      <c r="G33" s="2">
+        <v>161749.20000000001</v>
+      </c>
+      <c r="H33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2.1263888888861402</v>
+      </c>
+      <c r="E34" s="2">
+        <v>216838</v>
+      </c>
+      <c r="F34" s="2">
+        <v>198238.6</v>
+      </c>
+      <c r="G34" s="2">
+        <v>195867.6</v>
+      </c>
+      <c r="H34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="1">
+        <v>4.0749999999970896</v>
+      </c>
+      <c r="E35" s="2">
+        <v>237471.6</v>
+      </c>
+      <c r="F35" s="2">
+        <v>199825.2</v>
+      </c>
+      <c r="G35" s="2">
+        <v>184894.8</v>
+      </c>
+      <c r="H35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>7.0999999999985448</v>
+      </c>
+      <c r="E36" s="2">
+        <v>264293.59999999998</v>
+      </c>
+      <c r="F36" s="2">
+        <v>187605.6</v>
+      </c>
+      <c r="G36" s="2">
+        <v>200257.6</v>
+      </c>
+      <c r="H36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
         <v>7</v>
       </c>
-      <c r="D32">
-        <v>3</v>
-      </c>
-      <c r="E32" s="3">
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>98719.6</v>
+      </c>
+      <c r="F37" s="2">
+        <v>95160.2</v>
+      </c>
+      <c r="G37" s="2">
+        <v>104659</v>
+      </c>
+      <c r="H37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.22013888888614019</v>
+      </c>
+      <c r="E38" s="2">
+        <v>84123.4</v>
+      </c>
+      <c r="F38" s="2">
+        <v>75136.600000000006</v>
+      </c>
+      <c r="G38" s="2">
+        <v>99223</v>
+      </c>
+      <c r="H38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.49583333333430302</v>
+      </c>
+      <c r="E39" s="2">
+        <v>106857.60000000001</v>
+      </c>
+      <c r="F39" s="2">
+        <v>110985.4</v>
+      </c>
+      <c r="G39" s="2">
+        <v>132808.4</v>
+      </c>
+      <c r="H39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.9881944444423425</v>
+      </c>
+      <c r="E40" s="2">
+        <v>133345.60000000001</v>
+      </c>
+      <c r="F40" s="2">
+        <v>137744</v>
+      </c>
+      <c r="G40" s="2">
+        <v>168970.4</v>
+      </c>
+      <c r="H40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2.1263888888861402</v>
+      </c>
+      <c r="E41" s="2">
+        <v>179050</v>
+      </c>
+      <c r="F41" s="2">
+        <v>163774.6</v>
+      </c>
+      <c r="G41" s="2">
+        <v>205072</v>
+      </c>
+      <c r="H41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1">
+        <v>4.0749999999970896</v>
+      </c>
+      <c r="E42" s="2">
+        <v>211698.8</v>
+      </c>
+      <c r="F42" s="2">
+        <v>190657.6</v>
+      </c>
+      <c r="G42" s="2">
+        <v>211138.4</v>
+      </c>
+      <c r="H42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <v>7.0999999999985448</v>
+      </c>
+      <c r="E43" s="2">
+        <v>170996.8</v>
+      </c>
+      <c r="F43" s="2">
+        <v>133321.20000000001</v>
+      </c>
+      <c r="G43" s="2">
+        <v>146213.6</v>
+      </c>
+      <c r="H43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>32.517560929232246</v>
+      </c>
+      <c r="F44" s="3">
+        <v>31.569848726909015</v>
+      </c>
+      <c r="G44" s="3">
+        <v>29.987914014251345</v>
+      </c>
+      <c r="H44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.22013888888614019</v>
+      </c>
+      <c r="E45" s="3">
+        <v>177.33507782715219</v>
+      </c>
+      <c r="F45" s="3">
+        <v>178.98094596408873</v>
+      </c>
+      <c r="G45" s="3">
+        <v>162.785507853838</v>
+      </c>
+      <c r="H45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.49583333333430302</v>
+      </c>
+      <c r="E46" s="3">
+        <v>107.7330631891956</v>
+      </c>
+      <c r="F46" s="3">
+        <v>103.17777356395095</v>
+      </c>
+      <c r="G46" s="3">
+        <v>108.10037164190248</v>
+      </c>
+      <c r="H46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.9881944444423425</v>
+      </c>
+      <c r="E47" s="3">
+        <v>52.35138372647782</v>
+      </c>
+      <c r="F47" s="3">
+        <v>51.228826711620684</v>
+      </c>
+      <c r="G47" s="3">
+        <v>55.731415543140315</v>
+      </c>
+      <c r="H47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2.1263888888861402</v>
+      </c>
+      <c r="E48" s="3">
+        <v>59.722880184432029</v>
+      </c>
+      <c r="F48" s="3">
+        <v>60.79833766652871</v>
+      </c>
+      <c r="G48" s="3">
+        <v>59.160217355284772</v>
+      </c>
+      <c r="H48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="1">
+        <v>4.0749999999970896</v>
+      </c>
+      <c r="E49" s="3">
+        <v>72.744060432708977</v>
+      </c>
+      <c r="F49" s="3">
+        <v>68.866336044869058</v>
+      </c>
+      <c r="G49" s="3">
+        <v>69.17605375194168</v>
+      </c>
+      <c r="H49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <v>7.0999999999985448</v>
+      </c>
+      <c r="E50" s="3">
+        <v>55.363535287553304</v>
+      </c>
+      <c r="F50" s="3">
+        <v>47.838679734676361</v>
+      </c>
+      <c r="G50" s="3">
+        <v>49.598276915691713</v>
+      </c>
+      <c r="H50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+      <c r="E51" s="3">
+        <v>19.644190831782375</v>
+      </c>
+      <c r="F51" s="3">
+        <v>27.508879192945543</v>
+      </c>
+      <c r="G51" s="3">
         <v>17.966269729759794</v>
       </c>
-      <c r="F32" s="3">
+      <c r="H51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.22013888888614019</v>
+      </c>
+      <c r="E52" s="3">
+        <v>-32.431813256435021</v>
+      </c>
+      <c r="F52" s="3">
+        <v>-7.8933458560227336</v>
+      </c>
+      <c r="G52" s="3">
         <v>-30.338002991006533</v>
       </c>
-      <c r="G32" s="3">
+      <c r="H52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.49583333333430302</v>
+      </c>
+      <c r="E53" s="3">
+        <v>-32.235847570610247</v>
+      </c>
+      <c r="F53" s="3">
+        <v>-27.371462065310538</v>
+      </c>
+      <c r="G53" s="3">
         <v>-32.990201072747539</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H53" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.9881944444423425</v>
+      </c>
+      <c r="E54" s="3">
+        <v>-25.223472178409679</v>
+      </c>
+      <c r="F54" s="3">
+        <v>-24.881561856139854</v>
+      </c>
+      <c r="G54" s="3">
         <v>-25.217718025884437</v>
       </c>
-      <c r="I32" s="3">
+      <c r="H54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="1">
+        <v>2.1263888888861402</v>
+      </c>
+      <c r="E55" s="3">
+        <v>-35.296297536212876</v>
+      </c>
+      <c r="F55" s="3">
+        <v>-33.85599422746742</v>
+      </c>
+      <c r="G55" s="3">
         <v>-36.309981554197293</v>
       </c>
-      <c r="J32" s="3">
+      <c r="H55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="1">
+        <v>4.0749999999970896</v>
+      </c>
+      <c r="E56" s="3">
+        <v>33.955744488115272</v>
+      </c>
+      <c r="F56" s="3">
+        <v>22.526070565314484</v>
+      </c>
+      <c r="G56" s="3">
         <v>21.037077759739105</v>
       </c>
-      <c r="K32" s="3">
+      <c r="H56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57">
+        <v>7.0999999999985448</v>
+      </c>
+      <c r="E57" s="3">
+        <v>-11.600473912886457</v>
+      </c>
+      <c r="F57" s="3">
+        <v>-12.259599628150966</v>
+      </c>
+      <c r="G57" s="3">
         <v>-8.5438538529546122</v>
+      </c>
+      <c r="H57" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3545,8 +4170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EEE8FE-C703-DB49-A74A-F8C034F9931F}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3575,10 +4200,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>2</v>
@@ -3605,7 +4230,7 @@
         <v>7.1</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -3616,7 +4241,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -3646,7 +4271,7 @@
         <v>751000</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -3657,7 +4282,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -3695,7 +4320,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -3733,7 +4358,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4">
         <v>0.2</v>
@@ -3771,7 +4396,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4">
         <v>0.2</v>
@@ -3809,7 +4434,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="4">
         <v>0.2</v>
@@ -3847,7 +4472,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="4">
         <v>0.4</v>
@@ -3885,7 +4510,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="4">
         <v>0.4</v>
@@ -3923,7 +4548,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="4">
         <v>0.4</v>
@@ -3961,7 +4586,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4">
         <v>0.8</v>
@@ -3999,7 +4624,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="4">
         <v>0.8</v>
@@ -4037,7 +4662,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="4">
         <v>0.8</v>
@@ -4075,7 +4700,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="4">
         <v>1.6</v>
@@ -4113,7 +4738,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="4">
         <v>1.6</v>
@@ -4151,7 +4776,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="4">
         <v>1.6</v>
@@ -4189,7 +4814,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="4">
         <v>10</v>
@@ -4227,7 +4852,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="4">
         <v>10</v>
@@ -4265,7 +4890,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="4">
         <v>10</v>
@@ -4303,7 +4928,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="4">
         <v>0</v>
@@ -4341,7 +4966,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="4">
         <v>0</v>
@@ -4379,7 +5004,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="4">
         <v>0</v>
@@ -4417,7 +5042,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" s="4">
         <v>0.2</v>
@@ -4455,7 +5080,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="4">
         <v>0.2</v>
@@ -4493,7 +5118,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" s="4">
         <v>0.2</v>
@@ -4531,7 +5156,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27" s="4">
         <v>0.4</v>
@@ -4569,7 +5194,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" s="4">
         <v>0.4</v>
@@ -4607,7 +5232,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D29" s="4">
         <v>0.4</v>
@@ -4645,7 +5270,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" s="4">
         <v>0.8</v>
@@ -4683,7 +5308,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31" s="4">
         <v>0.8</v>
@@ -4721,7 +5346,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D32" s="4">
         <v>0.8</v>
@@ -4759,7 +5384,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D33" s="4">
         <v>10</v>
@@ -4797,7 +5422,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D34" s="4">
         <v>10</v>
@@ -4835,7 +5460,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="4">
         <v>10</v>

</xml_diff>